<commit_message>
Added cows and linked pages
</commit_message>
<xml_diff>
--- a/Documentation/GANTT.xlsx
+++ b/Documentation/GANTT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leones1\Desktop\Moocycle\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2A7D2E-878D-496A-AE17-E057E195A1D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3837CFFF-8571-4979-93B9-0ED18D2AA6FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" activeTab="1" xr2:uid="{82196E9E-969C-41C4-8C76-6F835B01D2A9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{82196E9E-969C-41C4-8C76-6F835B01D2A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Plannification" sheetId="1" r:id="rId1"/>
@@ -613,13 +613,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="13" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -646,24 +656,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="13" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F3D48B-8DED-4C7C-B631-681DE86B11D7}">
   <dimension ref="A1:AF54"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,157 +1003,157 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="53"/>
       <c r="C1" s="16"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="61"/>
+      <c r="X1" s="61"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="61"/>
+      <c r="AA1" s="61"/>
+      <c r="AB1" s="61"/>
     </row>
     <row r="2" spans="1:32" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="44" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="55">
+      <c r="D2" s="46">
         <v>45616</v>
       </c>
-      <c r="E2" s="55">
+      <c r="E2" s="46">
         <v>45623</v>
       </c>
-      <c r="F2" s="55">
+      <c r="F2" s="46">
         <v>45630</v>
       </c>
-      <c r="G2" s="55">
+      <c r="G2" s="46">
         <v>45637</v>
       </c>
-      <c r="H2" s="55">
+      <c r="H2" s="46">
         <v>45644</v>
       </c>
-      <c r="I2" s="55">
+      <c r="I2" s="46">
         <v>45651</v>
       </c>
-      <c r="J2" s="55">
+      <c r="J2" s="46">
         <v>45658</v>
       </c>
-      <c r="K2" s="55">
+      <c r="K2" s="46">
         <v>45665</v>
       </c>
-      <c r="L2" s="55">
+      <c r="L2" s="46">
         <v>45672</v>
       </c>
-      <c r="M2" s="55">
+      <c r="M2" s="46">
         <v>45679</v>
       </c>
-      <c r="N2" s="55">
+      <c r="N2" s="46">
         <v>45686</v>
       </c>
-      <c r="O2" s="55">
+      <c r="O2" s="46">
         <v>45693</v>
       </c>
-      <c r="P2" s="55">
+      <c r="P2" s="46">
         <v>45700</v>
       </c>
-      <c r="Q2" s="55">
+      <c r="Q2" s="46">
         <v>45707</v>
       </c>
-      <c r="R2" s="55">
+      <c r="R2" s="46">
         <v>45714</v>
       </c>
-      <c r="S2" s="55">
+      <c r="S2" s="46">
         <v>45721</v>
       </c>
-      <c r="T2" s="55">
+      <c r="T2" s="46">
         <v>45728</v>
       </c>
-      <c r="U2" s="55">
+      <c r="U2" s="46">
         <v>45735</v>
       </c>
-      <c r="V2" s="55">
+      <c r="V2" s="46">
         <v>45742</v>
       </c>
-      <c r="W2" s="55">
+      <c r="W2" s="46">
         <v>45749</v>
       </c>
-      <c r="X2" s="55">
+      <c r="X2" s="46">
         <v>45756</v>
       </c>
-      <c r="Y2" s="55">
+      <c r="Y2" s="46">
         <v>45763</v>
       </c>
-      <c r="Z2" s="55">
+      <c r="Z2" s="46">
         <v>45770</v>
       </c>
-      <c r="AA2" s="55">
+      <c r="AA2" s="46">
         <v>45777</v>
       </c>
-      <c r="AB2" s="55">
+      <c r="AB2" s="46">
         <v>45784</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="56"/>
-      <c r="T3" s="56"/>
-      <c r="U3" s="56"/>
-      <c r="V3" s="56"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="56"/>
-      <c r="Z3" s="56"/>
-      <c r="AA3" s="56"/>
-      <c r="AB3" s="56"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="47"/>
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="47"/>
+      <c r="X3" s="47"/>
+      <c r="Y3" s="47"/>
+      <c r="Z3" s="47"/>
+      <c r="AA3" s="47"/>
+      <c r="AB3" s="47"/>
     </row>
     <row r="4" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
@@ -1184,10 +1184,10 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="54"/>
+      <c r="C5" s="58"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
@@ -1222,31 +1222,31 @@
       <c r="C6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="58"/>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="58"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="58"/>
-      <c r="U6" s="58"/>
-      <c r="V6" s="58"/>
-      <c r="W6" s="58"/>
-      <c r="X6" s="58"/>
-      <c r="Y6" s="58"/>
-      <c r="Z6" s="58"/>
-      <c r="AA6" s="58"/>
-      <c r="AB6" s="59"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
+      <c r="V6" s="49"/>
+      <c r="W6" s="49"/>
+      <c r="X6" s="49"/>
+      <c r="Y6" s="49"/>
+      <c r="Z6" s="49"/>
+      <c r="AA6" s="49"/>
+      <c r="AB6" s="50"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
@@ -1516,7 +1516,7 @@
     </row>
     <row r="14" spans="1:32" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="32"/>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="45" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="6"/>
@@ -2153,7 +2153,7 @@
       <c r="AF30" s="2"/>
     </row>
     <row r="31" spans="1:32" s="4" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="50"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="21"/>
       <c r="C31" s="22"/>
       <c r="D31" s="21"/>
@@ -2187,7 +2187,7 @@
       <c r="AF31" s="21"/>
     </row>
     <row r="32" spans="1:32" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="10"/>
       <c r="C32" s="11"/>
       <c r="D32" s="13"/>
@@ -2221,7 +2221,7 @@
       <c r="AF32" s="2"/>
     </row>
     <row r="33" spans="1:32" s="4" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
+      <c r="A33" s="54"/>
       <c r="B33" s="21"/>
       <c r="C33" s="22"/>
       <c r="D33" s="21"/>
@@ -2255,7 +2255,7 @@
       <c r="AF33" s="21"/>
     </row>
     <row r="34" spans="1:32" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="50"/>
+      <c r="A34" s="54"/>
       <c r="B34" s="10"/>
       <c r="C34" s="11"/>
       <c r="D34" s="10"/>
@@ -2289,7 +2289,7 @@
       <c r="AF34" s="2"/>
     </row>
     <row r="35" spans="1:32" s="4" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="51"/>
+      <c r="A35" s="55"/>
       <c r="B35" s="23"/>
       <c r="C35" s="22"/>
       <c r="D35" s="21"/>
@@ -2323,7 +2323,7 @@
       <c r="AF35" s="21"/>
     </row>
     <row r="36" spans="1:32" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="51"/>
+      <c r="A36" s="55"/>
       <c r="B36" s="10"/>
       <c r="C36" s="11"/>
       <c r="D36" s="10"/>
@@ -2357,7 +2357,7 @@
       <c r="AF36" s="10"/>
     </row>
     <row r="37" spans="1:32" s="4" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="51"/>
+      <c r="A37" s="55"/>
       <c r="B37" s="21"/>
       <c r="C37" s="22"/>
       <c r="D37" s="21"/>
@@ -2391,7 +2391,7 @@
       <c r="AF37" s="21"/>
     </row>
     <row r="38" spans="1:32" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="51"/>
+      <c r="A38" s="55"/>
       <c r="B38" s="10"/>
       <c r="C38" s="11"/>
       <c r="D38" s="10"/>
@@ -2425,7 +2425,7 @@
       <c r="AF38" s="10"/>
     </row>
     <row r="39" spans="1:32" s="4" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="51"/>
+      <c r="A39" s="55"/>
       <c r="B39" s="21"/>
       <c r="C39" s="22"/>
       <c r="D39" s="21"/>
@@ -2459,7 +2459,7 @@
       <c r="AF39" s="21"/>
     </row>
     <row r="40" spans="1:32" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="51"/>
+      <c r="A40" s="55"/>
       <c r="B40" s="10"/>
       <c r="C40" s="11"/>
       <c r="D40" s="10"/>
@@ -2493,7 +2493,7 @@
       <c r="AF40" s="10"/>
     </row>
     <row r="41" spans="1:32" s="4" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="51"/>
+      <c r="A41" s="55"/>
       <c r="B41" s="21"/>
       <c r="C41" s="22"/>
       <c r="D41" s="21"/>
@@ -2527,7 +2527,7 @@
       <c r="AF41" s="21"/>
     </row>
     <row r="42" spans="1:32" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="47"/>
+      <c r="A42" s="51"/>
       <c r="B42" s="10"/>
       <c r="C42" s="11"/>
       <c r="D42" s="10"/>
@@ -2561,7 +2561,7 @@
       <c r="AF42" s="10"/>
     </row>
     <row r="43" spans="1:32" s="4" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="47"/>
+      <c r="A43" s="51"/>
       <c r="B43" s="21"/>
       <c r="C43" s="22"/>
       <c r="D43" s="21"/>
@@ -2595,7 +2595,7 @@
       <c r="AF43" s="21"/>
     </row>
     <row r="44" spans="1:32" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="47"/>
+      <c r="A44" s="51"/>
       <c r="B44" s="10"/>
       <c r="C44" s="11"/>
       <c r="D44" s="13"/>
@@ -2629,7 +2629,7 @@
       <c r="AF44" s="10"/>
     </row>
     <row r="45" spans="1:32" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="47"/>
+      <c r="A45" s="51"/>
       <c r="B45" s="10"/>
       <c r="C45" s="11"/>
       <c r="D45" s="10"/>
@@ -2660,7 +2660,7 @@
       <c r="AC45" s="10"/>
     </row>
     <row r="46" spans="1:32" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="47"/>
+      <c r="A46" s="51"/>
       <c r="B46" s="10"/>
       <c r="C46" s="11"/>
       <c r="D46" s="10"/>
@@ -2691,7 +2691,7 @@
       <c r="AC46" s="10"/>
     </row>
     <row r="47" spans="1:32" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="47"/>
+      <c r="A47" s="51"/>
       <c r="B47" s="10"/>
       <c r="C47" s="11"/>
       <c r="D47" s="10"/>
@@ -2939,6 +2939,31 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="S1:W1"/>
+    <mergeCell ref="X1:AB1"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="C2:C3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="AB2:AB3"/>
     <mergeCell ref="D6:AB6"/>
@@ -2955,31 +2980,6 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="I1:M1"/>
-    <mergeCell ref="N1:R1"/>
-    <mergeCell ref="S1:W1"/>
-    <mergeCell ref="X1:AB1"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -2990,8 +2990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C543C5B7-6436-42E3-B880-C082EEEC3E82}">
   <dimension ref="A1:AF53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="B4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3003,157 +3003,157 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="53"/>
       <c r="C1" s="16"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="61"/>
+      <c r="X1" s="61"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="61"/>
+      <c r="AA1" s="61"/>
+      <c r="AB1" s="61"/>
     </row>
     <row r="2" spans="1:32" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="44" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="55">
+      <c r="D2" s="46">
         <v>45616</v>
       </c>
-      <c r="E2" s="55">
+      <c r="E2" s="46">
         <v>45623</v>
       </c>
-      <c r="F2" s="55">
+      <c r="F2" s="46">
         <v>45630</v>
       </c>
-      <c r="G2" s="55">
+      <c r="G2" s="46">
         <v>45637</v>
       </c>
-      <c r="H2" s="55">
+      <c r="H2" s="46">
         <v>45644</v>
       </c>
-      <c r="I2" s="55">
+      <c r="I2" s="46">
         <v>45651</v>
       </c>
-      <c r="J2" s="55">
+      <c r="J2" s="46">
         <v>45658</v>
       </c>
-      <c r="K2" s="55">
+      <c r="K2" s="46">
         <v>45665</v>
       </c>
-      <c r="L2" s="55">
+      <c r="L2" s="46">
         <v>45672</v>
       </c>
-      <c r="M2" s="55">
+      <c r="M2" s="46">
         <v>45679</v>
       </c>
-      <c r="N2" s="55">
+      <c r="N2" s="46">
         <v>45686</v>
       </c>
-      <c r="O2" s="55">
+      <c r="O2" s="46">
         <v>45693</v>
       </c>
-      <c r="P2" s="55">
+      <c r="P2" s="46">
         <v>45700</v>
       </c>
-      <c r="Q2" s="55">
+      <c r="Q2" s="46">
         <v>45707</v>
       </c>
-      <c r="R2" s="55">
+      <c r="R2" s="46">
         <v>45714</v>
       </c>
-      <c r="S2" s="55">
+      <c r="S2" s="46">
         <v>45721</v>
       </c>
-      <c r="T2" s="55">
+      <c r="T2" s="46">
         <v>45728</v>
       </c>
-      <c r="U2" s="55">
+      <c r="U2" s="46">
         <v>45735</v>
       </c>
-      <c r="V2" s="55">
+      <c r="V2" s="46">
         <v>45742</v>
       </c>
-      <c r="W2" s="55">
+      <c r="W2" s="46">
         <v>45749</v>
       </c>
-      <c r="X2" s="55">
+      <c r="X2" s="46">
         <v>45756</v>
       </c>
-      <c r="Y2" s="55">
+      <c r="Y2" s="46">
         <v>45763</v>
       </c>
-      <c r="Z2" s="55">
+      <c r="Z2" s="46">
         <v>45770</v>
       </c>
-      <c r="AA2" s="55">
+      <c r="AA2" s="46">
         <v>45777</v>
       </c>
-      <c r="AB2" s="55">
+      <c r="AB2" s="46">
         <v>45784</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="56"/>
-      <c r="T3" s="56"/>
-      <c r="U3" s="56"/>
-      <c r="V3" s="56"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="56"/>
-      <c r="Z3" s="56"/>
-      <c r="AA3" s="56"/>
-      <c r="AB3" s="56"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="47"/>
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="47"/>
+      <c r="X3" s="47"/>
+      <c r="Y3" s="47"/>
+      <c r="Z3" s="47"/>
+      <c r="AA3" s="47"/>
+      <c r="AB3" s="47"/>
     </row>
     <row r="4" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
@@ -3184,10 +3184,10 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="54"/>
+      <c r="C5" s="58"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
@@ -3222,31 +3222,31 @@
       <c r="C6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="58"/>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="58"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="58"/>
-      <c r="U6" s="58"/>
-      <c r="V6" s="58"/>
-      <c r="W6" s="58"/>
-      <c r="X6" s="58"/>
-      <c r="Y6" s="58"/>
-      <c r="Z6" s="58"/>
-      <c r="AA6" s="58"/>
-      <c r="AB6" s="59"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
+      <c r="V6" s="49"/>
+      <c r="W6" s="49"/>
+      <c r="X6" s="49"/>
+      <c r="Y6" s="49"/>
+      <c r="Z6" s="49"/>
+      <c r="AA6" s="49"/>
+      <c r="AB6" s="50"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
@@ -3296,7 +3296,7 @@
       <c r="C8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="60"/>
+      <c r="D8" s="44"/>
       <c r="E8" s="2"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -3335,7 +3335,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="60"/>
+      <c r="E9" s="44"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -3411,7 +3411,7 @@
         <v>19</v>
       </c>
       <c r="D11" s="5"/>
-      <c r="E11" s="60"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
@@ -3449,7 +3449,7 @@
         <v>14</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="60"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -3516,12 +3516,12 @@
     </row>
     <row r="14" spans="1:32" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="32"/>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="45" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="60"/>
+      <c r="E14" s="44"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -3552,12 +3552,12 @@
     </row>
     <row r="15" spans="1:32" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32"/>
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="45" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="60"/>
+      <c r="E15" s="44"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -4113,7 +4113,7 @@
       <c r="AF29" s="2"/>
     </row>
     <row r="30" spans="1:32" s="4" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="21"/>
       <c r="C30" s="22"/>
       <c r="D30" s="21"/>
@@ -4147,7 +4147,7 @@
       <c r="AF30" s="21"/>
     </row>
     <row r="31" spans="1:32" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="50"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="10"/>
       <c r="C31" s="11"/>
       <c r="D31" s="13"/>
@@ -4181,7 +4181,7 @@
       <c r="AF31" s="2"/>
     </row>
     <row r="32" spans="1:32" s="4" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="21"/>
       <c r="C32" s="22"/>
       <c r="D32" s="21"/>
@@ -4215,7 +4215,7 @@
       <c r="AF32" s="21"/>
     </row>
     <row r="33" spans="1:32" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
+      <c r="A33" s="54"/>
       <c r="B33" s="10"/>
       <c r="C33" s="11"/>
       <c r="D33" s="10"/>
@@ -4249,7 +4249,7 @@
       <c r="AF33" s="2"/>
     </row>
     <row r="34" spans="1:32" s="4" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="51"/>
+      <c r="A34" s="55"/>
       <c r="B34" s="23"/>
       <c r="C34" s="22"/>
       <c r="D34" s="21"/>
@@ -4283,7 +4283,7 @@
       <c r="AF34" s="21"/>
     </row>
     <row r="35" spans="1:32" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="51"/>
+      <c r="A35" s="55"/>
       <c r="B35" s="10"/>
       <c r="C35" s="11"/>
       <c r="D35" s="10"/>
@@ -4317,7 +4317,7 @@
       <c r="AF35" s="10"/>
     </row>
     <row r="36" spans="1:32" s="4" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="51"/>
+      <c r="A36" s="55"/>
       <c r="B36" s="21"/>
       <c r="C36" s="22"/>
       <c r="D36" s="21"/>
@@ -4351,7 +4351,7 @@
       <c r="AF36" s="21"/>
     </row>
     <row r="37" spans="1:32" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="51"/>
+      <c r="A37" s="55"/>
       <c r="B37" s="10"/>
       <c r="C37" s="11"/>
       <c r="D37" s="10"/>
@@ -4385,7 +4385,7 @@
       <c r="AF37" s="10"/>
     </row>
     <row r="38" spans="1:32" s="4" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="51"/>
+      <c r="A38" s="55"/>
       <c r="B38" s="21"/>
       <c r="C38" s="22"/>
       <c r="D38" s="21"/>
@@ -4419,7 +4419,7 @@
       <c r="AF38" s="21"/>
     </row>
     <row r="39" spans="1:32" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="51"/>
+      <c r="A39" s="55"/>
       <c r="B39" s="10"/>
       <c r="C39" s="11"/>
       <c r="D39" s="10"/>
@@ -4453,7 +4453,7 @@
       <c r="AF39" s="10"/>
     </row>
     <row r="40" spans="1:32" s="4" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="51"/>
+      <c r="A40" s="55"/>
       <c r="B40" s="21"/>
       <c r="C40" s="22"/>
       <c r="D40" s="21"/>
@@ -4487,7 +4487,7 @@
       <c r="AF40" s="21"/>
     </row>
     <row r="41" spans="1:32" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="47"/>
+      <c r="A41" s="51"/>
       <c r="B41" s="10"/>
       <c r="C41" s="11"/>
       <c r="D41" s="10"/>
@@ -4521,7 +4521,7 @@
       <c r="AF41" s="10"/>
     </row>
     <row r="42" spans="1:32" s="4" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="47"/>
+      <c r="A42" s="51"/>
       <c r="B42" s="21"/>
       <c r="C42" s="22"/>
       <c r="D42" s="21"/>
@@ -4555,7 +4555,7 @@
       <c r="AF42" s="21"/>
     </row>
     <row r="43" spans="1:32" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="47"/>
+      <c r="A43" s="51"/>
       <c r="B43" s="10"/>
       <c r="C43" s="11"/>
       <c r="D43" s="13"/>
@@ -4589,7 +4589,7 @@
       <c r="AF43" s="10"/>
     </row>
     <row r="44" spans="1:32" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="47"/>
+      <c r="A44" s="51"/>
       <c r="B44" s="10"/>
       <c r="C44" s="11"/>
       <c r="D44" s="10"/>
@@ -4620,7 +4620,7 @@
       <c r="AC44" s="10"/>
     </row>
     <row r="45" spans="1:32" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="47"/>
+      <c r="A45" s="51"/>
       <c r="B45" s="10"/>
       <c r="C45" s="11"/>
       <c r="D45" s="10"/>
@@ -4651,7 +4651,7 @@
       <c r="AC45" s="10"/>
     </row>
     <row r="46" spans="1:32" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="47"/>
+      <c r="A46" s="51"/>
       <c r="B46" s="10"/>
       <c r="C46" s="11"/>
       <c r="D46" s="10"/>
@@ -4899,12 +4899,25 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="X1:AB1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="I1:M1"/>
-    <mergeCell ref="N1:R1"/>
-    <mergeCell ref="S1:W1"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
     <mergeCell ref="D6:AB6"/>
     <mergeCell ref="T2:T3"/>
     <mergeCell ref="U2:U3"/>
@@ -4921,25 +4934,12 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="X1:AB1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="S1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -4947,6 +4947,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A44DCC2B49D54A4DAA68A1B63285C88B" ma:contentTypeVersion="4" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="55aa73dc9b0ee9079bb7d1d4af7f2271">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="27a3f57d-59ce-4168-8277-ddfca740493d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5754e39b53a0f22b99f1c1409831c365" ns2:_="">
     <xsd:import namespace="27a3f57d-59ce-4168-8277-ddfca740493d"/>
@@ -5090,12 +5096,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5106,6 +5106,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46A33A18-0DE2-4AE2-925C-3D8B5B543F80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A7FCB2E-3CC2-4B5D-A4CA-AACD67EF51D4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5123,15 +5132,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46A33A18-0DE2-4AE2-925C-3D8B5B543F80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67790079-2CD3-4C6C-BC5A-A92A87166551}">
   <ds:schemaRefs>

</xml_diff>